<commit_message>
adicionado CNPJ e IP
</commit_message>
<xml_diff>
--- a/dados_ini.xlsx
+++ b/dados_ini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,25 +436,30 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Arquivo</t>
+          <t>Empresa</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Empresa</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Operador</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Operador</t>
+          <t>CNPJ</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Porta</t>
         </is>
@@ -463,25 +468,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\ewertonc\CliSisTef.ini</t>
+          <t>VITO0166</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>VITO0166</t>
+          <t>CX000555</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CX000555</t>
+          <t>FXLXAXVXIOXxB</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>FXLXAXVXIOXxB</t>
+          <t>313333395000141</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
+        <is>
+          <t>555.55.555.53</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>COM99</t>
         </is>
@@ -490,25 +500,30 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\ewertonc\CliSisTef.ini</t>
+          <t>VITO0166</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>VITO0166</t>
+          <t>CX000555</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CX000555</t>
+          <t>FXLXAXVXIOXxB</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>FXLXAXVXIOXxB</t>
+          <t>313333395000141</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
+        <is>
+          <t>555.55.555.53</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>COM99</t>
         </is>
@@ -517,25 +532,30 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\ewertonc\CliSisTef.ini</t>
+          <t>VITO0166</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VITO0166</t>
+          <t>CX000555</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CX000555</t>
+          <t>FXLXAXVXIOXxB</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>FXLXAXVXIOXxB</t>
+          <t>313333395000141</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
+        <is>
+          <t>555.55.555.53</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>COM99</t>
         </is>
@@ -544,25 +564,30 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\ewertonc\CliSisTef.ini</t>
+          <t>VITO0166</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VITO0166</t>
+          <t>CX000555</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CX000555</t>
+          <t>FXLXAXVXIOXxB</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>FXLXAXVXIOXxB</t>
+          <t>313333395000141</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
+        <is>
+          <t>555.55.555.53</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>COM99</t>
         </is>
@@ -571,25 +596,30 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\ewertonc\CliSisTef.ini</t>
+          <t>VITO0166</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>VITO0166</t>
+          <t>CX000555</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CX000555</t>
+          <t>FXLXAXVXIOXxB</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FXLXAXVXIOXxB</t>
+          <t>313333395000141</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>555.55.555.53</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>COM99</t>
         </is>
@@ -598,25 +628,30 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\ewertonc\CliSisTef.ini</t>
+          <t>VITO0166</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>VITO0166</t>
+          <t>CX000555</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CX000555</t>
+          <t>FXLXAXVXIOXxB</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FXLXAXVXIOXxB</t>
+          <t>313333395000141</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>555.55.555.53</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>COM99</t>
         </is>
@@ -625,25 +660,30 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\flaviob\CliSiTef.ini</t>
+          <t>VITO0141</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>VITO0141</t>
+          <t>CX000001</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CX000001</t>
+          <t>ALCIDES</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ALCIDES</t>
+          <t>31371695000141</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>172.27.221.53</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>COM9</t>
         </is>
@@ -652,25 +692,30 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\flaviob\CliSiTef.ini</t>
+          <t>VITO0141</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>VITO0141</t>
+          <t>CX000001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CX000001</t>
+          <t>ALCIDES</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ALCIDES</t>
+          <t>31371695000141</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
+        <is>
+          <t>172.27.221.53</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>COM9</t>
         </is>
@@ -679,25 +724,30 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\flaviob\CliSiTef.ini</t>
+          <t>VITO0141</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>VITO0141</t>
+          <t>CX000001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CX000001</t>
+          <t>ALCIDES</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>ALCIDES</t>
+          <t>31371695000141</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>172.27.221.53</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>COM9</t>
         </is>
@@ -706,25 +756,30 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\flaviob\CliSiTef.ini</t>
+          <t>VITO0141</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>VITO0141</t>
+          <t>CX000001</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CX000001</t>
+          <t>ALCIDES</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ALCIDES</t>
+          <t>31371695000141</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>172.27.221.53</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>COM9</t>
         </is>
@@ -733,25 +788,30 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\flaviob\CliSiTef.ini</t>
+          <t>VITO0141</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>VITO0141</t>
+          <t>CX000001</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CX000001</t>
+          <t>ALCIDES</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>ALCIDES</t>
+          <t>31371695000141</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>172.27.221.53</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>COM9</t>
         </is>
@@ -760,25 +820,30 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>C:\Users\dti.flaviob\Desktop\Estrutura\VM00213\flaviob\CliSiTef.ini</t>
+          <t>VITO0141</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>VITO0141</t>
+          <t>CX000001</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CX000001</t>
+          <t>ALCIDES</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ALCIDES</t>
+          <t>31371695000141</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
+        <is>
+          <t>172.27.221.53</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
         <is>
           <t>COM9</t>
         </is>

</xml_diff>